<commit_message>
add modified raw excel data and modify the BTEX_compound_plotting and acceptors_compound_plotting for better quality figures
</commit_message>
<xml_diff>
--- a/data/raw/CW_field_meassurements/Raw_data_lab/240120_Resultaten_ronde_T3.xlsx
+++ b/data/raw/CW_field_meassurements/Raw_data_lab/240120_Resultaten_ronde_T3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\raw\CW_field_meassurements\Raw_data_Anne_Marie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\raw\CW_field_meassurements\Raw_data_lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72B4799C-8E81-4ECB-9581-960E1F94212B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB25F7BF-DEF3-4E43-AAC3-B7F761A91E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="532">
   <si>
     <t>Analysis</t>
   </si>
@@ -939,12 +939,6 @@
     <t>14243903-002</t>
   </si>
   <si>
-    <t>CW1_EFF(CW1_EFF-1-4)</t>
-  </si>
-  <si>
-    <t>INF(INF-1-4)</t>
-  </si>
-  <si>
     <t>2025-02-25</t>
   </si>
   <si>
@@ -1047,21 +1041,6 @@
     <t>14243904-005</t>
   </si>
   <si>
-    <t>CW1MF01(CW1MF01-1-5)</t>
-  </si>
-  <si>
-    <t>CW1MF02(CW1MF02-1-5)</t>
-  </si>
-  <si>
-    <t>CW1MF05(CW1MF05-1-4)</t>
-  </si>
-  <si>
-    <t>CW1MF06(CW1MF06-1-4)</t>
-  </si>
-  <si>
-    <t>CW1MF10(CW1MF10-1-5)</t>
-  </si>
-  <si>
     <t>9,9</t>
   </si>
   <si>
@@ -1200,27 +1179,6 @@
     <t>14244713-007</t>
   </si>
   <si>
-    <t>CW1MF09(CW1MF09-1-5)</t>
-  </si>
-  <si>
-    <t>CW2MF01(CW2MF01-1-4)</t>
-  </si>
-  <si>
-    <t>CW2MF02(CW2MF02-1-4)</t>
-  </si>
-  <si>
-    <t>CW2MF05(CW2MF05-1-4)</t>
-  </si>
-  <si>
-    <t>CW2MF06(CW2MF06-1-4)</t>
-  </si>
-  <si>
-    <t>CW2MF09(CW2MF09-1-4)</t>
-  </si>
-  <si>
-    <t>CW2MF10(CW2MF10-1-4)</t>
-  </si>
-  <si>
     <t>2025-02-28</t>
   </si>
   <si>
@@ -1362,9 +1320,6 @@
     <t>14244714-001</t>
   </si>
   <si>
-    <t>CW2_EFF(CW2_EFF-1-5)</t>
-  </si>
-  <si>
     <t>2025-02-26</t>
   </si>
   <si>
@@ -1404,24 +1359,6 @@
     <t>14245611-006</t>
   </si>
   <si>
-    <t>CW3MF01(CW3MF01-1-4)</t>
-  </si>
-  <si>
-    <t>CW3MF02(CW3MF02-1-4)</t>
-  </si>
-  <si>
-    <t>CW3MF05(CW3MF05-1-4)</t>
-  </si>
-  <si>
-    <t>CW3MF06(CW3MF06-1-4)</t>
-  </si>
-  <si>
-    <t>CW3MF09(CW3MF09-1-4)</t>
-  </si>
-  <si>
-    <t>CW3MF10(CW3MF10-1-4)</t>
-  </si>
-  <si>
     <t>2025-02-27</t>
   </si>
   <si>
@@ -1536,9 +1473,6 @@
     <t>14245613-001</t>
   </si>
   <si>
-    <t>CW3_EFF(CW3_EFF-1-4)</t>
-  </si>
-  <si>
     <t>1924</t>
   </si>
   <si>
@@ -1690,6 +1624,12 @@
   </si>
   <si>
     <t>1899-12-30T13:59:35</t>
+  </si>
+  <si>
+    <t>nitriet-N</t>
+  </si>
+  <si>
+    <t>nitraa-N</t>
   </si>
 </sst>
 </file>
@@ -2107,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:X62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2130,64 +2070,64 @@
         <v>300</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -2337,70 +2277,70 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>301</v>
+        <v>483</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>302</v>
+        <v>528</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>337</v>
+        <v>486</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>338</v>
+        <v>488</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>339</v>
+        <v>490</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>340</v>
+        <v>492</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>341</v>
+        <v>497</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>388</v>
+        <v>494</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>389</v>
+        <v>501</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>390</v>
+        <v>503</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>391</v>
+        <v>505</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>392</v>
+        <v>507</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>393</v>
+        <v>509</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>394</v>
+        <v>511</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>442</v>
+        <v>499</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>456</v>
+        <v>516</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>457</v>
+        <v>518</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>458</v>
+        <v>520</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>459</v>
+        <v>522</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>460</v>
+        <v>524</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>461</v>
+        <v>526</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>500</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -2550,70 +2490,70 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -2621,70 +2561,70 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -2698,10 +2638,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>17</v>
@@ -2719,7 +2659,7 @@
         <v>15</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>15</v>
@@ -2734,7 +2674,7 @@
         <v>15</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>16</v>
@@ -2743,19 +2683,19 @@
         <v>16</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="W12" s="3" t="s">
         <v>15</v>
@@ -2772,7 +2712,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>18</v>
@@ -2784,7 +2724,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>15</v>
@@ -2793,7 +2733,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>15</v>
@@ -2808,7 +2748,7 @@
         <v>15</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>16</v>
@@ -2823,7 +2763,7 @@
         <v>57</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="U13" s="3" t="s">
         <v>15</v>
@@ -2857,10 +2797,10 @@
         <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
@@ -2878,13 +2818,13 @@
         <v>182</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>88</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>19</v>
@@ -2905,7 +2845,7 @@
         <v>44</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="V15" s="3" t="s">
         <v>35</v>
@@ -2914,7 +2854,7 @@
         <v>33</v>
       </c>
       <c r="X15" s="3" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -2925,7 +2865,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>40</v>
@@ -2937,7 +2877,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>39</v>
@@ -2952,10 +2892,10 @@
         <v>36</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>31</v>
@@ -2976,13 +2916,13 @@
         <v>46</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="U16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="W16" s="3" t="s">
         <v>32</v>
@@ -3004,7 +2944,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>37</v>
@@ -3013,13 +2953,13 @@
         <v>88</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>88</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>88</v>
@@ -3240,25 +3180,25 @@
         <v>70</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>97</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>135</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>105</v>
@@ -3267,25 +3207,25 @@
         <v>121</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="V22" s="3" t="s">
         <v>109</v>
@@ -3356,7 +3296,7 @@
         <v>120</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>228</v>
@@ -3388,7 +3328,7 @@
         <v>94</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>98</v>
@@ -3397,13 +3337,13 @@
         <v>94</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>92</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>80</v>
@@ -3418,7 +3358,7 @@
         <v>74</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>72</v>
@@ -3427,19 +3367,19 @@
         <v>71</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="T24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="X24" s="3" t="s">
         <v>121</v>
@@ -3453,7 +3393,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>116</v>
@@ -3504,7 +3444,7 @@
         <v>104</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="U25" s="3" t="s">
         <v>93</v>
@@ -3539,7 +3479,7 @@
         <v>103</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>93</v>
@@ -3551,13 +3491,13 @@
         <v>142</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>114</v>
@@ -3566,13 +3506,13 @@
         <v>112</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>99</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>71</v>
@@ -3604,16 +3544,16 @@
         <v>216</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>111</v>
@@ -3622,16 +3562,16 @@
         <v>114</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>75</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>70</v>
@@ -3646,19 +3586,19 @@
         <v>94</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="S27" s="3" t="s">
         <v>77</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="U27" s="3" t="s">
         <v>71</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="W27" s="3" t="s">
         <v>116</v>
@@ -3675,70 +3615,70 @@
         <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="S28" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="X28" s="3" t="s">
         <v>479</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="U28" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="V28" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="W28" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="X28" s="3" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -3752,7 +3692,7 @@
         <v>185</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>128</v>
@@ -3764,10 +3704,10 @@
         <v>129</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>136</v>
@@ -3800,10 +3740,10 @@
         <v>183</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="V29" s="3" t="s">
         <v>107</v>
@@ -3831,52 +3771,52 @@
         <v>101</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>172</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>183</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>184</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>149</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>205</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="T31" s="3" t="s">
         <v>100</v>
@@ -3902,13 +3842,13 @@
         <v>53</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>99</v>
@@ -3926,13 +3866,13 @@
         <v>61</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>68</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>83</v>
@@ -3941,10 +3881,10 @@
         <v>61</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>137</v>
@@ -3976,13 +3916,13 @@
         <v>53</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>79</v>
@@ -4000,19 +3940,19 @@
         <v>145</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>61</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="P33" s="3" t="s">
         <v>83</v>
@@ -4033,7 +3973,7 @@
         <v>112</v>
       </c>
       <c r="V33" s="3" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
       <c r="W33" s="3" t="s">
         <v>93</v>
@@ -4065,10 +4005,10 @@
         <v>152</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>166</v>
@@ -4089,22 +4029,22 @@
         <v>159</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>153</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="T34" s="3" t="s">
         <v>153</v>
       </c>
       <c r="U34" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="V34" s="3" t="s">
         <v>159</v>
@@ -4113,7 +4053,7 @@
         <v>107</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -4136,7 +4076,7 @@
         <v>216</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>56</v>
@@ -4169,10 +4109,10 @@
         <v>34</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="T35" s="3" t="s">
         <v>160</v>
@@ -4184,10 +4124,10 @@
         <v>162</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -4198,16 +4138,16 @@
         <v>53</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>160</v>
@@ -4231,7 +4171,7 @@
         <v>160</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="O36" s="3" t="s">
         <v>160</v>
@@ -4278,10 +4218,10 @@
         <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>160</v>
@@ -4299,7 +4239,7 @@
         <v>160</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="M37" s="3" t="s">
         <v>160</v>
@@ -4326,7 +4266,7 @@
         <v>160</v>
       </c>
       <c r="U37" s="3" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="V37" s="3" t="s">
         <v>160</v>
@@ -4346,7 +4286,7 @@
         <v>53</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>35</v>
@@ -4361,7 +4301,7 @@
         <v>172</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>169</v>
@@ -4373,7 +4313,7 @@
         <v>172</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M38" s="3" t="s">
         <v>172</v>
@@ -4394,13 +4334,13 @@
         <v>172</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="T38" s="3" t="s">
         <v>172</v>
       </c>
       <c r="U38" s="3" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
       <c r="V38" s="3" t="s">
         <v>172</v>
@@ -4447,7 +4387,7 @@
         <v>160</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>160</v>
@@ -4571,7 +4511,7 @@
         <v>172</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>172</v>
@@ -4645,7 +4585,7 @@
         <v>160</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>160</v>
@@ -4719,7 +4659,7 @@
         <v>160</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>160</v>
@@ -4867,7 +4807,7 @@
         <v>160</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>160</v>
@@ -4941,7 +4881,7 @@
         <v>160</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>160</v>
@@ -5015,22 +4955,22 @@
         <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>186</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>156</v>
@@ -5039,7 +4979,7 @@
         <v>184</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="M47" s="3" t="s">
         <v>16</v>
@@ -5054,13 +4994,13 @@
         <v>133</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="T47" s="3" t="s">
         <v>100</v>
@@ -5075,7 +5015,7 @@
         <v>132</v>
       </c>
       <c r="X47" s="3" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -5086,70 +5026,70 @@
         <v>53</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>158</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="N48" s="3" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="T48" s="3" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="V48" s="3" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="W48" s="3" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="X48" s="3" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -5171,10 +5111,10 @@
         <v>195</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>133</v>
@@ -5186,28 +5126,28 @@
         <v>210</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="M50" s="3" t="s">
         <v>194</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>210</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="R50" s="3" t="s">
         <v>94</v>
@@ -5225,10 +5165,10 @@
         <v>87</v>
       </c>
       <c r="W50" s="3" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="X50" s="3" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
@@ -5242,7 +5182,7 @@
         <v>116</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>218</v>
@@ -5263,10 +5203,10 @@
         <v>194</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="M51" s="3" t="s">
         <v>194</v>
@@ -5464,28 +5404,28 @@
         <v>138</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>208</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>133</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>195</v>
@@ -5494,37 +5434,37 @@
         <v>26</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="P54" s="3" t="s">
         <v>211</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="R54" s="3" t="s">
         <v>68</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="T54" s="3" t="s">
         <v>209</v>
       </c>
       <c r="U54" s="3" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="V54" s="3" t="s">
         <v>142</v>
       </c>
       <c r="W54" s="3" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="X54" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -5543,22 +5483,22 @@
         <v>216</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>218</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>219</v>
@@ -5567,7 +5507,7 @@
         <v>219</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="M56" s="3" t="s">
         <v>87</v>
@@ -5682,7 +5622,7 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>530</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>222</v>
@@ -5830,7 +5770,7 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>223</v>
+        <v>531</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>222</v>
@@ -5913,16 +5853,16 @@
         <v>41</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>95</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>144</v>
@@ -5943,7 +5883,7 @@
         <v>118</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="O61" s="3" t="s">
         <v>90</v>
@@ -6155,13 +6095,13 @@
         <v>268</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>505</v>
+        <v>483</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>507</v>
+        <v>485</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
@@ -6225,13 +6165,13 @@
         <v>268</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>508</v>
+        <v>486</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>509</v>
+        <v>487</v>
       </c>
       <c r="H3" s="6">
         <v>0</v>
@@ -6295,13 +6235,13 @@
         <v>268</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>510</v>
+        <v>488</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>511</v>
+        <v>489</v>
       </c>
       <c r="H4" s="6">
         <v>0</v>
@@ -6365,13 +6305,13 @@
         <v>268</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>513</v>
+        <v>491</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
@@ -6435,13 +6375,13 @@
         <v>268</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>515</v>
+        <v>493</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -6502,13 +6442,13 @@
         <v>268</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>516</v>
+        <v>494</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>518</v>
+        <v>496</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>269</v>
@@ -6569,13 +6509,13 @@
         <v>268</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>519</v>
+        <v>497</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>520</v>
+        <v>498</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -6639,13 +6579,13 @@
         <v>268</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>522</v>
+        <v>500</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>269</v>
@@ -6706,13 +6646,13 @@
         <v>268</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>523</v>
+        <v>501</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>524</v>
+        <v>502</v>
       </c>
       <c r="H10" s="6">
         <v>0</v>
@@ -6776,13 +6716,13 @@
         <v>268</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>525</v>
+        <v>503</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>526</v>
+        <v>504</v>
       </c>
       <c r="H11" s="6">
         <v>0</v>
@@ -6846,13 +6786,13 @@
         <v>268</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>527</v>
+        <v>505</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>528</v>
+        <v>506</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>269</v>
@@ -6913,13 +6853,13 @@
         <v>268</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>529</v>
+        <v>507</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>530</v>
+        <v>508</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>269</v>
@@ -6980,13 +6920,13 @@
         <v>268</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>531</v>
+        <v>509</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>269</v>
@@ -7047,13 +6987,13 @@
         <v>268</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>269</v>
@@ -7114,13 +7054,13 @@
         <v>268</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>269</v>
@@ -7181,13 +7121,13 @@
         <v>268</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>539</v>
+        <v>517</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>269</v>
@@ -7248,13 +7188,13 @@
         <v>268</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>269</v>
@@ -7315,13 +7255,13 @@
         <v>268</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>543</v>
+        <v>521</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>269</v>
@@ -7382,13 +7322,13 @@
         <v>268</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>544</v>
+        <v>522</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>269</v>
@@ -7446,13 +7386,13 @@
         <v>268</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>546</v>
+        <v>524</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>269</v>
@@ -7513,13 +7453,13 @@
         <v>268</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>548</v>
+        <v>526</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>549</v>
+        <v>527</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>269</v>
@@ -7580,13 +7520,13 @@
         <v>268</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>550</v>
+        <v>528</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>551</v>
+        <v>529</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>269</v>

</xml_diff>